<commit_message>
Add more models evaluation results
</commit_message>
<xml_diff>
--- a/Evaluation Result/xlsx/Evaluation.xlsx
+++ b/Evaluation Result/xlsx/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\Learned-Image-Compression\Evaluation Result\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44403AB-0072-4846-AE82-F1AEC224CF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1168133-08AE-4D56-A5EC-D21898C69013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15098" yWindow="-4358" windowWidth="15196" windowHeight="23476" tabRatio="868" firstSheet="6" activeTab="12" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="868" activeTab="13" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
   </bookViews>
   <sheets>
     <sheet name="Factorized" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,12 @@
     <sheet name="ELIC2022" sheetId="10" r:id="rId7"/>
     <sheet name="CNN2022" sheetId="19" r:id="rId8"/>
     <sheet name="STF2022" sheetId="20" r:id="rId9"/>
-    <sheet name="TCM2023" sheetId="32" r:id="rId10"/>
-    <sheet name="MLIC2023" sheetId="36" r:id="rId11"/>
-    <sheet name="CCA2024" sheetId="33" r:id="rId12"/>
-    <sheet name="FLIC2025" sheetId="35" r:id="rId13"/>
+    <sheet name="Inv2022" sheetId="37" r:id="rId10"/>
+    <sheet name="TCM2023" sheetId="32" r:id="rId11"/>
+    <sheet name="MLIC2023" sheetId="36" r:id="rId12"/>
+    <sheet name="CCA2024" sheetId="33" r:id="rId13"/>
+    <sheet name="WeConvene2024" sheetId="38" r:id="rId14"/>
+    <sheet name="FLIC2025" sheetId="35" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="15">
   <si>
     <t>Δms-ssim</t>
   </si>
@@ -494,8 +496,8 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G42" sqref="G42"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -886,6 +888,402 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CFCE91-4782-4DDF-AF34-A9F809908C8E}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.1089386666666667</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.1893526635443171</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8.0413996877650426E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>27.743573427200321</v>
+      </c>
+      <c r="F2" s="2">
+        <v>28.679769833882649</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.93619640668233117</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.91289333750804269</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.93153662234544754</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.864328483740485E-2</v>
+      </c>
+      <c r="K2" s="6">
+        <v>155.43046732545869</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.36358938924968243</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.41622020552555722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.14683733333333329</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.22818853085239729</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8.1351197519063972E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>28.75411454836528</v>
+      </c>
+      <c r="F3" s="2">
+        <v>29.578843990961708</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.82472944259643555</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.93071475625038147</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.94426256914933526</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.3547812898953789E-2</v>
+      </c>
+      <c r="K3" s="6">
+        <v>120.11132533568509</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.31242719727257889</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.38004250824451452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.177648</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.25956662620107329</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8.1918626201073319E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>29.513434092203781</v>
+      </c>
+      <c r="F4" s="2">
+        <v>30.221535205841061</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.70810111363728723</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.94181634982426965</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.95197829107443488</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.016194125016523E-2</v>
+      </c>
+      <c r="K4" s="6">
+        <v>99.642928454101479</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.27616044009725249</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.35009410729010898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.31437333333333328</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.38933979533612728</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.4966462002793943E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>31.682770490646359</v>
+      </c>
+      <c r="F5" s="2">
+        <v>32.170896609624229</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.48812611897786701</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.96576477835575736</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.97003938754399621</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4.2746091882388537E-3</v>
+      </c>
+      <c r="K5" s="6">
+        <v>59.997134884791251</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.18682703856999669</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.27442194769779837</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.48128533333333318</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.59125924110412598</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.1099739077707928</v>
+      </c>
+      <c r="E6" s="2">
+        <v>33.686023076375328</v>
+      </c>
+      <c r="F6" s="2">
+        <v>34.137340227762863</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.45131715138752782</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.97781090190013253</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.98020108292500174</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.390181024869209E-3</v>
+      </c>
+      <c r="K6" s="6">
+        <v>38.62854403866811</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.13428535413307449</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.21636451780796051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.69202133333333349</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.79042769099275267</v>
+      </c>
+      <c r="D7" s="3">
+        <v>9.8406357659419186E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>35.570674419403083</v>
+      </c>
+      <c r="F7" s="2">
+        <v>35.894662062327058</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.32398764292398852</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.98562148213386536</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.98686328281958902</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.2418006857236601E-3</v>
+      </c>
+      <c r="K7" s="6">
+        <v>25.114041972788751</v>
+      </c>
+      <c r="L7" s="6">
+        <v>9.4641360609481737E-2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.1645571514964104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.84254933333333326</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.93196949486931169</v>
+      </c>
+      <c r="D8" s="3">
+        <v>8.9420161535978426E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>36.648180325826011</v>
+      </c>
+      <c r="F8" s="2">
+        <v>36.891103744506843</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.24292341868082451</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.98889605204264319</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.98960400372743607</v>
+      </c>
+      <c r="J8" s="3">
+        <v>7.0795168479287351E-4</v>
+      </c>
+      <c r="K8" s="6">
+        <v>17.642206879425089</v>
+      </c>
+      <c r="L8" s="6">
+        <v>7.6955689932219684E-2</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0.1389616057276726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>0.09</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.1345706666666671</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.209233527382215</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.4662860715548174E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>38.221662203470864</v>
+      </c>
+      <c r="F9" s="2">
+        <v>38.369090716044113</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.14742851257324219</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.99240465710560477</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.99277117103338242</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3.6651392777764519E-4</v>
+      </c>
+      <c r="K9" s="6">
+        <v>11.48015925429655</v>
+      </c>
+      <c r="L9" s="6">
+        <v>5.5845719412900507E-2</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0.1043237174550692</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C9FCE1-5B75-43BC-8AA1-33EC73BA8665}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1200,7 +1598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76679E6B-2391-4BC2-9D4A-2012A92B30DB}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1514,7 +1912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97ADBE1-D45B-4C85-B278-2E9475F30FD7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1757,12 +2155,326 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928D4A31-A2DF-4F2E-8426-1E762FDC96C0}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.17790400000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.99880520502726233</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.82090120502726238</v>
+      </c>
+      <c r="E2" s="2">
+        <v>29.897226969401039</v>
+      </c>
+      <c r="F2" s="2">
+        <v>29.895416021347049</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.810948053996952E-3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.94552753120660782</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.94552678118149436</v>
+      </c>
+      <c r="J2" s="3">
+        <v>7.500251134606728E-7</v>
+      </c>
+      <c r="K2" s="6">
+        <v>89.755966678339632</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.24688549526035791</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.32735025137662888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.22089600000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.046746179461479</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.82585017946147921</v>
+      </c>
+      <c r="E3" s="2">
+        <v>30.684243758519489</v>
+      </c>
+      <c r="F3" s="2">
+        <v>30.682327508926392</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.9162495930977741E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.95503117144107819</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.95503062754869461</v>
+      </c>
+      <c r="J3" s="3">
+        <v>5.4389238357543945E-7</v>
+      </c>
+      <c r="K3" s="6">
+        <v>75.134669537063701</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.2147997822612524</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.29965940862894058</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.33161066666666678</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.165398508310318</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.83378784164365127</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32.325033744176231</v>
+      </c>
+      <c r="F4" s="2">
+        <v>32.322654247283943</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.3794968922956632E-3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.96932870646317804</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.96932982156674063</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.1151035625989181E-6</v>
+      </c>
+      <c r="K4" s="6">
+        <v>50.0238698080002</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.15737342989693079</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.24382304151852929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.48192000000000002</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.3175273487965271</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.83560734879652676</v>
+      </c>
+      <c r="E5" s="2">
+        <v>34.062723318735763</v>
+      </c>
+      <c r="F5" s="2">
+        <v>34.059029817581177</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.6935011545793368E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.97948671380678809</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.97948555399974191</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.159807046180461E-6</v>
+      </c>
+      <c r="K5" s="6">
+        <v>31.601149184835322</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.114179892387862</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.19179878632227579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.67824533333333326</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.512098719676336</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.83385338634300232</v>
+      </c>
+      <c r="E6" s="2">
+        <v>35.790611426035561</v>
+      </c>
+      <c r="F6" s="2">
+        <v>35.785048802693687</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5.5626233418735183E-3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.98608545958995819</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.98608386516571045</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.594424247741699E-6</v>
+      </c>
+      <c r="K6" s="6">
+        <v>20.808660047216559</v>
+      </c>
+      <c r="L6" s="6">
+        <v>8.3658138561683401E-2</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.14919789880514139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.95747733333333329</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.783284311493238</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.82580697815990445</v>
+      </c>
+      <c r="E7" s="2">
+        <v>37.697122255961098</v>
+      </c>
+      <c r="F7" s="2">
+        <v>37.68920691808065</v>
+      </c>
+      <c r="G7" s="3">
+        <v>7.915337880447737E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.99074602872133255</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.99074343591928482</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.5928020477294922E-6</v>
+      </c>
+      <c r="K7" s="6">
+        <v>13.65504975859915</v>
+      </c>
+      <c r="L7" s="6">
+        <v>5.8662204362917691E-2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.1093827212850253</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C627A75-F734-49B6-86FE-0E2F8BE2BA01}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2880,7 +3592,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
@@ -3277,7 +3989,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G37" sqref="G37"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4532,7 +5244,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Rectify a year error
</commit_message>
<xml_diff>
--- a/Evaluation Result/xlsx/Evaluation.xlsx
+++ b/Evaluation Result/xlsx/Evaluation.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\Learned-Image-Compression\Evaluation Result\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1168133-08AE-4D56-A5EC-D21898C69013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994FB421-33A9-4CFB-A8D5-7264A7525B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="868" activeTab="13" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="868" activeTab="15" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
   </bookViews>
   <sheets>
     <sheet name="Factorized" sheetId="1" r:id="rId1"/>
     <sheet name="Hyperprior" sheetId="3" r:id="rId2"/>
-    <sheet name="Mbt2018-mean" sheetId="5" r:id="rId3"/>
-    <sheet name="Mbt2018" sheetId="9" r:id="rId4"/>
-    <sheet name="Cheng2020Anchor" sheetId="7" r:id="rId5"/>
-    <sheet name="Cheng2020Attn" sheetId="12" r:id="rId6"/>
-    <sheet name="ELIC2022" sheetId="10" r:id="rId7"/>
-    <sheet name="CNN2022" sheetId="19" r:id="rId8"/>
-    <sheet name="STF2022" sheetId="20" r:id="rId9"/>
-    <sheet name="Inv2022" sheetId="37" r:id="rId10"/>
-    <sheet name="TCM2023" sheetId="32" r:id="rId11"/>
-    <sheet name="MLIC2023" sheetId="36" r:id="rId12"/>
-    <sheet name="CCA2024" sheetId="33" r:id="rId13"/>
-    <sheet name="WeConvene2024" sheetId="38" r:id="rId14"/>
-    <sheet name="FLIC2025" sheetId="35" r:id="rId15"/>
+    <sheet name="Mbt2018-mean-ste" sheetId="38" r:id="rId3"/>
+    <sheet name="Mbt2018-mean" sheetId="5" r:id="rId4"/>
+    <sheet name="Mbt2018" sheetId="9" r:id="rId5"/>
+    <sheet name="Cheng2020Anchor" sheetId="7" r:id="rId6"/>
+    <sheet name="Cheng2020Attn" sheetId="12" r:id="rId7"/>
+    <sheet name="ELIC2022" sheetId="10" r:id="rId8"/>
+    <sheet name="CNN2022" sheetId="19" r:id="rId9"/>
+    <sheet name="STF2022" sheetId="20" r:id="rId10"/>
+    <sheet name="Inv2022" sheetId="37" r:id="rId11"/>
+    <sheet name="TCM2023" sheetId="32" r:id="rId12"/>
+    <sheet name="MLIC2023" sheetId="36" r:id="rId13"/>
+    <sheet name="CCA2024" sheetId="33" r:id="rId14"/>
+    <sheet name="WeConvene2024" sheetId="39" r:id="rId15"/>
+    <sheet name="FTIC2024" sheetId="35" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="18">
   <si>
     <t>Δms-ssim</t>
   </si>
@@ -98,6 +99,15 @@
   <si>
     <t>Δpsnr</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DISTS</t>
+  </si>
+  <si>
+    <t>LPIPS</t>
+  </si>
+  <si>
+    <t>FID</t>
   </si>
 </sst>
 </file>
@@ -888,6 +898,321 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF49183C-33BC-4E63-A6B9-E2DC80E0439F}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1.8E-3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.12690133333333331</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.39428266013662022</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.26738132680328691</v>
+      </c>
+      <c r="E2" s="2">
+        <v>28.59163928031921</v>
+      </c>
+      <c r="F2" s="2">
+        <v>28.603989124298099</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.2349843978881839E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.92776427169640863</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.92775911341110862</v>
+      </c>
+      <c r="J2" s="3">
+        <v>5.1582853000109452E-6</v>
+      </c>
+      <c r="K2" s="6">
+        <v>110.92377417964281</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.30211931467056269</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.37158926328023267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.20002666666666671</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.47060780972242361</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.27058114305575692</v>
+      </c>
+      <c r="E3" s="2">
+        <v>30.058413982391361</v>
+      </c>
+      <c r="F3" s="2">
+        <v>30.069785515467331</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.137153307596961E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.95005122075478232</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.95032760749260581</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2.7638673782348627E-4</v>
+      </c>
+      <c r="K3" s="6">
+        <v>76.455145219948292</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.2337548534075419</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.31469186147054029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.32413333333333327</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.59438745925823844</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.27025412592490511</v>
+      </c>
+      <c r="E4" s="2">
+        <v>31.827214320500691</v>
+      </c>
+      <c r="F4" s="2">
+        <v>31.814417044321701</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.27972761789934E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.96731578061978019</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.96706617623567581</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2.496043841043738E-4</v>
+      </c>
+      <c r="K4" s="6">
+        <v>48.826156190084362</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.1655846734841665</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.25176887214183807</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.49489599999999989</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.76805337394277251</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.27315737394277262</v>
+      </c>
+      <c r="E5" s="2">
+        <v>33.643482287724822</v>
+      </c>
+      <c r="F5" s="2">
+        <v>33.642379363377891</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.1029243469238279E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.9782085195183754</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.97825515518585837</v>
+      </c>
+      <c r="J5" s="3">
+        <v>4.6635667482974867E-5</v>
+      </c>
+      <c r="K5" s="6">
+        <v>31.786889240879422</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.11891970038414</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.19771166642506921</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.68746666666666678</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.95138428856929147</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.26391762190262469</v>
+      </c>
+      <c r="E6" s="2">
+        <v>35.428832372029618</v>
+      </c>
+      <c r="F6" s="2">
+        <v>35.382302761077881</v>
+      </c>
+      <c r="G6" s="3">
+        <v>4.6529610951743898E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.98525741696357727</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.98520226528247201</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5.515168110525881E-5</v>
+      </c>
+      <c r="K6" s="6">
+        <v>20.342729227864709</v>
+      </c>
+      <c r="L6" s="6">
+        <v>8.3819319804509476E-2</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.1518293445309003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.96591999999999978</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.218432987729708</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.25251298772970859</v>
+      </c>
+      <c r="E7" s="2">
+        <v>37.319753011067711</v>
+      </c>
+      <c r="F7" s="2">
+        <v>37.283927917480469</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.5825093587241952E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.99004207303126657</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.9900256569186846</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.641611258196285E-5</v>
+      </c>
+      <c r="K7" s="6">
+        <v>12.49797422669479</v>
+      </c>
+      <c r="L7" s="6">
+        <v>6.0202623407045998E-2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.11295463889837271</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CFCE91-4782-4DDF-AF34-A9F809908C8E}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -1283,7 +1608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C9FCE1-5B75-43BC-8AA1-33EC73BA8665}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1598,7 +1923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76679E6B-2391-4BC2-9D4A-2012A92B30DB}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1912,7 +2237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97ADBE1-D45B-4C85-B278-2E9475F30FD7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -2155,12 +2480,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928D4A31-A2DF-4F2E-8426-1E762FDC96C0}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAFC1D9-C422-4B82-B16B-D889D0222DE2}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2469,12 +2794,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C627A75-F734-49B6-86FE-0E2F8BE2BA01}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3188,6 +3513,145 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744B61C1-8357-454C-BE0F-605C0340693E}">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="B2">
+        <v>0.159104</v>
+      </c>
+      <c r="C2">
+        <v>0.30343994311988348</v>
+      </c>
+      <c r="D2">
+        <v>0.14433594311988349</v>
+      </c>
+      <c r="E2">
+        <v>28.143000046412151</v>
+      </c>
+      <c r="F2">
+        <v>28.32690278689067</v>
+      </c>
+      <c r="G2">
+        <v>0.1839027404785156</v>
+      </c>
+      <c r="H2">
+        <v>0.92384535074234009</v>
+      </c>
+      <c r="I2">
+        <v>0.92540520429611206</v>
+      </c>
+      <c r="J2">
+        <v>1.5598535537719731E-3</v>
+      </c>
+      <c r="K2">
+        <v>110.49837618713281</v>
+      </c>
+      <c r="L2">
+        <v>0.32268826166788739</v>
+      </c>
+      <c r="M2">
+        <v>0.37496660898129153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1.6100000000000001E-3</v>
+      </c>
+      <c r="B3">
+        <v>0.15359999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.29559288173913961</v>
+      </c>
+      <c r="D3">
+        <v>0.14199288173913949</v>
+      </c>
+      <c r="E3">
+        <v>28.229444265365601</v>
+      </c>
+      <c r="F3">
+        <v>27.979055484135941</v>
+      </c>
+      <c r="G3">
+        <v>0.25038878122965608</v>
+      </c>
+      <c r="H3">
+        <v>0.92492032051086426</v>
+      </c>
+      <c r="I3">
+        <v>0.92181806017955148</v>
+      </c>
+      <c r="J3">
+        <v>3.1022603313127779E-3</v>
+      </c>
+      <c r="K3">
+        <v>109.6410637837439</v>
+      </c>
+      <c r="L3">
+        <v>0.31777926969031489</v>
+      </c>
+      <c r="M3">
+        <v>0.37836939593156182</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F434A9-C39C-4B85-AD7D-CCFD28D640D2}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -3587,7 +4051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62E5D48-6E06-4282-AC81-17F7FD3DD5D0}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -3983,7 +4447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D0977A-5C4A-4DEB-836B-5C1A72FD00E4}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -4327,7 +4791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF71C97-B095-4C2E-A3EC-E6044A9FA708}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -4671,7 +5135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB8A61D-3EA8-4BBB-9246-E018E6EA153F}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -5006,7 +5470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59202079-AD42-4F5C-8E99-21070582FC6A}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -5237,319 +5701,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF49183C-33BC-4E63-A6B9-E2DC80E0439F}">
-  <dimension ref="A1:M7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1.8E-3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.12690133333333331</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.39428266013662022</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.26738132680328691</v>
-      </c>
-      <c r="E2" s="2">
-        <v>28.59163928031921</v>
-      </c>
-      <c r="F2" s="2">
-        <v>28.603989124298099</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1.2349843978881839E-2</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.92776427169640863</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.92775911341110862</v>
-      </c>
-      <c r="J2" s="3">
-        <v>5.1582853000109452E-6</v>
-      </c>
-      <c r="K2" s="6">
-        <v>110.92377417964281</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0.30211931467056269</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0.37158926328023267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.20002666666666671</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.47060780972242361</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.27058114305575692</v>
-      </c>
-      <c r="E3" s="2">
-        <v>30.058413982391361</v>
-      </c>
-      <c r="F3" s="2">
-        <v>30.069785515467331</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1.137153307596961E-2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.95005122075478232</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.95032760749260581</v>
-      </c>
-      <c r="J3" s="3">
-        <v>2.7638673782348627E-4</v>
-      </c>
-      <c r="K3" s="6">
-        <v>76.455145219948292</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.2337548534075419</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.31469186147054029</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>6.7000000000000002E-3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.32413333333333327</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.59438745925823844</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.27025412592490511</v>
-      </c>
-      <c r="E4" s="2">
-        <v>31.827214320500691</v>
-      </c>
-      <c r="F4" s="2">
-        <v>31.814417044321701</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1.27972761789934E-2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.96731578061978019</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.96706617623567581</v>
-      </c>
-      <c r="J4" s="3">
-        <v>2.496043841043738E-4</v>
-      </c>
-      <c r="K4" s="6">
-        <v>48.826156190084362</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.1655846734841665</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0.25176887214183807</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.49489599999999989</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.76805337394277251</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.27315737394277262</v>
-      </c>
-      <c r="E5" s="2">
-        <v>33.643482287724822</v>
-      </c>
-      <c r="F5" s="2">
-        <v>33.642379363377891</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.1029243469238279E-3</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.9782085195183754</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.97825515518585837</v>
-      </c>
-      <c r="J5" s="3">
-        <v>4.6635667482974867E-5</v>
-      </c>
-      <c r="K5" s="6">
-        <v>31.786889240879422</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0.11891970038414</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0.19771166642506921</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.68746666666666678</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.95138428856929147</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.26391762190262469</v>
-      </c>
-      <c r="E6" s="2">
-        <v>35.428832372029618</v>
-      </c>
-      <c r="F6" s="2">
-        <v>35.382302761077881</v>
-      </c>
-      <c r="G6" s="3">
-        <v>4.6529610951743898E-2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.98525741696357727</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.98520226528247201</v>
-      </c>
-      <c r="J6" s="3">
-        <v>5.515168110525881E-5</v>
-      </c>
-      <c r="K6" s="6">
-        <v>20.342729227864709</v>
-      </c>
-      <c r="L6" s="6">
-        <v>8.3819319804509476E-2</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0.1518293445309003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>4.8300000000000003E-2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.96591999999999978</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.218432987729708</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.25251298772970859</v>
-      </c>
-      <c r="E7" s="2">
-        <v>37.319753011067711</v>
-      </c>
-      <c r="F7" s="2">
-        <v>37.283927917480469</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3.5825093587241952E-2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.99004207303126657</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.9900256569186846</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1.641611258196285E-5</v>
-      </c>
-      <c r="K7" s="6">
-        <v>12.49797422669479</v>
-      </c>
-      <c r="L7" s="6">
-        <v>6.0202623407045998E-2</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0.11295463889837271</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix some lambda value error
</commit_message>
<xml_diff>
--- a/Evaluation Result/xlsx/Evaluation.xlsx
+++ b/Evaluation Result/xlsx/Evaluation.xlsx
@@ -8,28 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\Learned-Image-Compression\Evaluation Result\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF7D93F-454D-45C7-9253-3D5EFACDED37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB7826F-7E3C-49B6-80F5-A134D200FBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="868" activeTab="7" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="868" activeTab="15" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
   </bookViews>
   <sheets>
     <sheet name="Factorized" sheetId="1" r:id="rId1"/>
     <sheet name="Hyperprior" sheetId="3" r:id="rId2"/>
-    <sheet name="Mbt2018-mean-ste" sheetId="38" r:id="rId3"/>
-    <sheet name="Mbt2018-mean" sheetId="5" r:id="rId4"/>
-    <sheet name="Mbt2018" sheetId="9" r:id="rId5"/>
-    <sheet name="Cheng2020Anchor" sheetId="7" r:id="rId6"/>
-    <sheet name="Cheng2020Attn" sheetId="12" r:id="rId7"/>
-    <sheet name="DPICT2022" sheetId="40" r:id="rId8"/>
-    <sheet name="ELIC2022" sheetId="10" r:id="rId9"/>
-    <sheet name="CNN2022" sheetId="19" r:id="rId10"/>
-    <sheet name="STF2022" sheetId="20" r:id="rId11"/>
-    <sheet name="Inv2022" sheetId="37" r:id="rId12"/>
-    <sheet name="TCM2023" sheetId="32" r:id="rId13"/>
-    <sheet name="MLIC2023" sheetId="36" r:id="rId14"/>
-    <sheet name="CCA2024" sheetId="33" r:id="rId15"/>
-    <sheet name="WeConvene2024" sheetId="39" r:id="rId16"/>
-    <sheet name="FTIC2024" sheetId="35" r:id="rId17"/>
+    <sheet name="Mbt2018-mean" sheetId="5" r:id="rId3"/>
+    <sheet name="Mbt2018" sheetId="9" r:id="rId4"/>
+    <sheet name="Cheng2020Anchor" sheetId="7" r:id="rId5"/>
+    <sheet name="Cheng2020Attn" sheetId="12" r:id="rId6"/>
+    <sheet name="DPICT2022" sheetId="40" r:id="rId7"/>
+    <sheet name="ELIC2022" sheetId="10" r:id="rId8"/>
+    <sheet name="CNN2022" sheetId="19" r:id="rId9"/>
+    <sheet name="STF2022" sheetId="20" r:id="rId10"/>
+    <sheet name="Inv2022" sheetId="37" r:id="rId11"/>
+    <sheet name="TCM2023" sheetId="32" r:id="rId12"/>
+    <sheet name="MLIC2023" sheetId="36" r:id="rId13"/>
+    <sheet name="CCA2024" sheetId="33" r:id="rId14"/>
+    <sheet name="WeConvene2024" sheetId="39" r:id="rId15"/>
+    <sheet name="FTIC2024" sheetId="35" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="183">
   <si>
     <t>Δms-ssim</t>
   </si>
@@ -100,12 +99,6 @@
   <si>
     <t>Δpsnr</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DISTS</t>
-  </si>
-  <si>
-    <t>LPIPS</t>
   </si>
   <si>
     <t>FID</t>
@@ -1015,7 +1008,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1072,7 +1065,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B2" s="2">
         <v>0.1380213333333333</v>
@@ -1113,7 +1106,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B3" s="2">
         <v>0.20905599999999999</v>
@@ -1154,7 +1147,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="B4" s="2">
         <v>0.31559999999999999</v>
@@ -1195,7 +1188,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>3.2000000000000002E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B5" s="2">
         <v>0.47880533333333308</v>
@@ -1236,7 +1229,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B6" s="2">
         <v>0.6990133333333336</v>
@@ -1277,7 +1270,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="B7" s="2">
         <v>1.03864</v>
@@ -1318,7 +1311,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>0.03</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="B8" s="2">
         <v>1.445930666666666</v>
@@ -1359,7 +1352,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>0.18</v>
       </c>
       <c r="B9" s="2">
         <v>1.9641919999999999</v>
@@ -1406,239 +1399,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59202079-AD42-4F5C-8E99-21070582FC6A}">
-  <dimension ref="A1:M5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA51" sqref="AA51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1.8E-3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0.1415733333333333</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0.37627519542972249</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.23470186209638921</v>
-      </c>
-      <c r="E2" s="2">
-        <v>29.014907360076901</v>
-      </c>
-      <c r="F2" s="2">
-        <v>29.01263125737508</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2.2761027018241009E-3</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.93290496369202935</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.93289164702097571</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1.331667105364254E-5</v>
-      </c>
-      <c r="K2" s="6">
-        <v>112.79812878575019</v>
-      </c>
-      <c r="L2" s="6">
-        <v>0.28842345873514807</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0.36777948091427493</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.218496</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.45518568033973378</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.23668968033973381</v>
-      </c>
-      <c r="E3" s="2">
-        <v>30.542146682739261</v>
-      </c>
-      <c r="F3" s="2">
-        <v>30.538185516993209</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3.9611657460518757E-3</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.95307789742946625</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.95306503772735596</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1.2859702110290531E-5</v>
-      </c>
-      <c r="K3" s="6">
-        <v>81.505320350226839</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0.22515885035196939</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.31315292914708448</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>6.7000000000000002E-3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.32326933333333341</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.55609557777643204</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.23282624444309871</v>
-      </c>
-      <c r="E4" s="2">
-        <v>32.069103717803962</v>
-      </c>
-      <c r="F4" s="2">
-        <v>32.06329027811686</v>
-      </c>
-      <c r="G4" s="3">
-        <v>5.8134396870954666E-3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.96799124032258987</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.96797890961170197</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1.2330710887908941E-5</v>
-      </c>
-      <c r="K4" s="6">
-        <v>53.088313848355369</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0.16271258393923441</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0.25484423339366907</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.69234133333333314</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.90979902197917306</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.21745768864583989</v>
-      </c>
-      <c r="E5" s="2">
-        <v>35.652261098225907</v>
-      </c>
-      <c r="F5" s="2">
-        <v>35.640590826670334</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1.1670271555587419E-2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0.98580639561017358</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.98580269267161691</v>
-      </c>
-      <c r="J5" s="3">
-        <v>3.702938556671143E-6</v>
-      </c>
-      <c r="K5" s="6">
-        <v>21.816504512335481</v>
-      </c>
-      <c r="L5" s="6">
-        <v>8.5436006387074784E-2</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0.154677485426267</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF49183C-33BC-4E63-A6B9-E2DC80E0439F}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -1953,12 +1713,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CFCE91-4782-4DDF-AF34-A9F809908C8E}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="V58" sqref="V58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2349,7 +2109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C9FCE1-5B75-43BC-8AA1-33EC73BA8665}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -2664,7 +2424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76679E6B-2391-4BC2-9D4A-2012A92B30DB}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -2978,7 +2738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97ADBE1-D45B-4C85-B278-2E9475F30FD7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -3221,7 +2981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAFC1D9-C422-4B82-B16B-D889D0222DE2}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -3535,12 +3295,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C627A75-F734-49B6-86FE-0E2F8BE2BA01}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W47" sqref="W47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3855,7 +3615,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3912,7 +3672,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B2" s="2">
         <v>0.15070933333333331</v>
@@ -3954,7 +3714,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B3" s="2">
         <v>0.23565333333333341</v>
@@ -3996,7 +3756,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="B4" s="2">
         <v>0.35615466666666667</v>
@@ -4038,7 +3798,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>3.2000000000000002E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B5" s="2">
         <v>0.52473599999999987</v>
@@ -4080,7 +3840,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B6" s="2">
         <v>0.7298186666666665</v>
@@ -4122,7 +3882,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="B7" s="2">
         <v>1.0210399999999999</v>
@@ -4164,7 +3924,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>0.03</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="B8" s="2">
         <v>1.367248</v>
@@ -4206,7 +3966,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>0.18</v>
       </c>
       <c r="B9" s="2">
         <v>1.8</v>
@@ -4254,151 +4014,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744B61C1-8357-454C-BE0F-605C0340693E}">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="B2">
-        <v>0.159104</v>
-      </c>
-      <c r="C2">
-        <v>0.30343994311988348</v>
-      </c>
-      <c r="D2">
-        <v>0.14433594311988349</v>
-      </c>
-      <c r="E2">
-        <v>28.143000046412151</v>
-      </c>
-      <c r="F2">
-        <v>28.32690278689067</v>
-      </c>
-      <c r="G2">
-        <v>0.1839027404785156</v>
-      </c>
-      <c r="H2">
-        <v>0.92384535074234009</v>
-      </c>
-      <c r="I2">
-        <v>0.92540520429611206</v>
-      </c>
-      <c r="J2">
-        <v>1.5598535537719731E-3</v>
-      </c>
-      <c r="K2">
-        <v>110.49837618713281</v>
-      </c>
-      <c r="L2">
-        <v>0.32268826166788739</v>
-      </c>
-      <c r="M2">
-        <v>0.37496660898129153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1.6100000000000001E-3</v>
-      </c>
-      <c r="B3">
-        <v>0.15359999999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.29559288173913961</v>
-      </c>
-      <c r="D3">
-        <v>0.14199288173913949</v>
-      </c>
-      <c r="E3">
-        <v>28.229444265365601</v>
-      </c>
-      <c r="F3">
-        <v>27.979055484135941</v>
-      </c>
-      <c r="G3">
-        <v>0.25038878122965608</v>
-      </c>
-      <c r="H3">
-        <v>0.92492032051086426</v>
-      </c>
-      <c r="I3">
-        <v>0.92181806017955148</v>
-      </c>
-      <c r="J3">
-        <v>3.1022603313127779E-3</v>
-      </c>
-      <c r="K3">
-        <v>109.6410637837439</v>
-      </c>
-      <c r="L3">
-        <v>0.31777926969031489</v>
-      </c>
-      <c r="M3">
-        <v>0.37836939593156182</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F434A9-C39C-4B85-AD7D-CCFD28D640D2}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4456,7 +4077,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B2" s="2">
         <v>0.14585066666666671</v>
@@ -4497,7 +4118,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B3" s="2">
         <v>0.2255573333333333</v>
@@ -4538,7 +4159,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="B4" s="2">
         <v>0.34348800000000002</v>
@@ -4579,7 +4200,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>3.2000000000000002E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B5" s="2">
         <v>0.50744533333333341</v>
@@ -4620,7 +4241,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B6" s="2">
         <v>0.72341333333333335</v>
@@ -4661,7 +4282,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="B7" s="2">
         <v>0.99429333333333303</v>
@@ -4705,7 +4326,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>0.03</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="B8" s="2">
         <v>1.3411679999999999</v>
@@ -4746,7 +4367,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>0.18</v>
       </c>
       <c r="B9" s="2">
         <v>1.761317333333333</v>
@@ -4792,13 +4413,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62E5D48-6E06-4282-AC81-17F7FD3DD5D0}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4855,7 +4476,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>4.0000000000000002E-4</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B2" s="2">
         <v>0.12446933333333331</v>
@@ -4896,7 +4517,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>8.0000000000000004E-4</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B3" s="2">
         <v>0.2084053333333333</v>
@@ -4937,7 +4558,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="B4" s="2">
         <v>0.31643733333333329</v>
@@ -4978,7 +4599,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>3.2000000000000002E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B5" s="2">
         <v>0.47154133333333342</v>
@@ -5019,7 +4640,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B6" s="2">
         <v>0.69166400000000017</v>
@@ -5060,7 +4681,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="B7" s="2">
         <v>0.95491199999999987</v>
@@ -5101,7 +4722,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>0.03</v>
+        <v>9.3200000000000005E-2</v>
       </c>
       <c r="B8" s="2">
         <v>1.2945333333333331</v>
@@ -5142,7 +4763,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>0.18</v>
       </c>
       <c r="B9" s="2">
         <v>1.7114240000000001</v>
@@ -5188,13 +4809,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D0977A-5C4A-4DEB-836B-5C1A72FD00E4}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5251,7 +4872,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B2" s="2">
         <v>0.132912</v>
@@ -5292,7 +4913,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>3.2000000000000002E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B3" s="2">
         <v>0.201712</v>
@@ -5333,7 +4954,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="B4" s="2">
         <v>0.29388266666666668</v>
@@ -5374,7 +4995,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B5" s="2">
         <v>0.450544</v>
@@ -5415,7 +5036,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B6" s="2">
         <v>0.63713066666666662</v>
@@ -5456,7 +5077,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="B7" s="2">
         <v>0.86271466666666674</v>
@@ -5532,13 +5153,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF71C97-B095-4C2E-A3EC-E6044A9FA708}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5595,7 +5216,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>1.8E-3</v>
       </c>
       <c r="B2" s="2">
         <v>0.12940266666666669</v>
@@ -5636,7 +5257,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>3.2000000000000002E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B3" s="2">
         <v>0.1921066666666667</v>
@@ -5677,7 +5298,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>6.7000000000000002E-3</v>
       </c>
       <c r="B4" s="2">
         <v>0.29208533333333331</v>
@@ -5718,7 +5339,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="B5" s="2">
         <v>0.46134399999999998</v>
@@ -5759,7 +5380,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B6" s="2">
         <v>0.63974933333333339</v>
@@ -5800,7 +5421,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="B7" s="2">
         <v>0.86411733333333318</v>
@@ -5876,11 +5497,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91AAE27A-2114-49A4-AA30-6CEE8CC95C9B}">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -5894,13 +5515,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>11</v>
@@ -5909,12 +5530,12 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" s="8">
         <v>1.46026611328125E-2</v>
@@ -5937,7 +5558,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" s="8">
         <v>1.6291300455729098E-2</v>
@@ -5960,7 +5581,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" s="8">
         <v>1.6571044921875E-2</v>
@@ -5983,7 +5604,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" s="8">
         <v>1.6820271809895801E-2</v>
@@ -6006,7 +5627,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" s="8">
         <v>1.751708984375E-2</v>
@@ -6029,7 +5650,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B7" s="8">
         <v>1.9612630208333301E-2</v>
@@ -6052,7 +5673,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B8" s="8">
         <v>2.1387736002604098E-2</v>
@@ -6075,7 +5696,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B9" s="8">
         <v>2.2603352864583301E-2</v>
@@ -6098,7 +5719,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B10" s="8">
         <v>2.3442586263020801E-2</v>
@@ -6121,7 +5742,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11" s="8">
         <v>2.4103800455729098E-2</v>
@@ -6144,7 +5765,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B12" s="8">
         <v>2.4586995442708301E-2</v>
@@ -6167,7 +5788,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B13" s="8">
         <v>2.5004069010416598E-2</v>
@@ -6190,7 +5811,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" s="8">
         <v>2.5370279947916598E-2</v>
@@ -6213,7 +5834,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B15" s="8">
         <v>2.5716145833333301E-2</v>
@@ -6236,7 +5857,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B16" s="8">
         <v>2.6000976562499899E-2</v>
@@ -6259,7 +5880,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B17" s="8">
         <v>2.6290893554687399E-2</v>
@@ -6282,7 +5903,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18" s="8">
         <v>2.6540120442708301E-2</v>
@@ -6305,7 +5926,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B19" s="8">
         <v>2.6799519856770801E-2</v>
@@ -6328,7 +5949,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B20" s="8">
         <v>2.7048746744791598E-2</v>
@@ -6351,7 +5972,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B21" s="8">
         <v>2.7292887369791598E-2</v>
@@ -6374,7 +5995,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B22" s="8">
         <v>3.2007853190104102E-2</v>
@@ -6397,7 +6018,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B23" s="8">
         <v>4.1737874348958301E-2</v>
@@ -6420,7 +6041,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B24" s="8">
         <v>4.9428304036458301E-2</v>
@@ -6443,7 +6064,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B25" s="8">
         <v>5.5180867513020801E-2</v>
@@ -6466,7 +6087,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B26" s="8">
         <v>5.914306640625E-2</v>
@@ -6489,7 +6110,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27" s="8">
         <v>6.18743896484375E-2</v>
@@ -6512,7 +6133,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B28" s="8">
         <v>6.3695271809895801E-2</v>
@@ -6535,7 +6156,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B29" s="8">
         <v>6.49566650390625E-2</v>
@@ -6558,7 +6179,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B30" s="8">
         <v>6.5882364908854102E-2</v>
@@ -6581,7 +6202,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B31" s="8">
         <v>6.65130615234375E-2</v>
@@ -6604,7 +6225,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B32" s="8">
         <v>6.7072550455729102E-2</v>
@@ -6627,7 +6248,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B33" s="8">
         <v>6.7494710286458301E-2</v>
@@ -6650,7 +6271,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B34" s="8">
         <v>6.7799886067708301E-2</v>
@@ -6673,7 +6294,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B35" s="8">
         <v>6.8089803059895801E-2</v>
@@ -6696,7 +6317,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B36" s="8">
         <v>6.83441162109375E-2</v>
@@ -6719,7 +6340,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B37" s="8">
         <v>6.85882568359375E-2</v>
@@ -6742,7 +6363,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B38" s="8">
         <v>7.69805908203125E-2</v>
@@ -6765,7 +6386,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B39" s="8">
         <v>9.5184326171875E-2</v>
@@ -6788,7 +6409,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B40" s="8">
         <v>0.112289428710937</v>
@@ -6811,7 +6432,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B41" s="8">
         <v>0.12827046712239501</v>
@@ -6834,7 +6455,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B42" s="8">
         <v>0.14296976725260399</v>
@@ -6857,7 +6478,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B43" s="8">
         <v>0.156402587890625</v>
@@ -6880,7 +6501,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B44" s="8">
         <v>0.16849263509114501</v>
@@ -6903,7 +6524,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B45" s="8">
         <v>0.179168701171875</v>
@@ -6926,7 +6547,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B46" s="8">
         <v>0.18856302897135399</v>
@@ -6949,7 +6570,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B47" s="8">
         <v>0.19690450032552001</v>
@@ -6972,7 +6593,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B48" s="8">
         <v>0.204132080078125</v>
@@ -6995,7 +6616,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B49" s="8">
         <v>0.210342407226562</v>
@@ -7018,7 +6639,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B50" s="8">
         <v>0.21576436360677001</v>
@@ -7041,7 +6662,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B51" s="8">
         <v>0.22033182779947899</v>
@@ -7064,7 +6685,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B52" s="8">
         <v>0.22424825032552001</v>
@@ -7087,7 +6708,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B53" s="8">
         <v>0.227508544921875</v>
@@ -7110,7 +6731,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B54" s="8">
         <v>0.23023478190104099</v>
@@ -7133,7 +6754,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B55" s="8">
         <v>0.23250834147135399</v>
@@ -7156,7 +6777,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B56" s="8">
         <v>0.23438008626302001</v>
@@ -7179,7 +6800,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B57" s="8">
         <v>0.23596700032552001</v>
@@ -7202,7 +6823,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B58" s="8">
         <v>0.23729960123697899</v>
@@ -7225,7 +6846,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B59" s="8">
         <v>0.23834228515625</v>
@@ -7248,7 +6869,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B60" s="8">
         <v>0.239227294921874</v>
@@ -7271,7 +6892,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B61" s="8">
         <v>0.23994954427083301</v>
@@ -7294,7 +6915,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B62" s="8">
         <v>0.24055989583333301</v>
@@ -7317,7 +6938,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B63" s="8">
         <v>0.24110921223958301</v>
@@ -7340,7 +6961,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B64" s="8">
         <v>0.24152628580729099</v>
@@ -7363,7 +6984,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B65" s="8">
         <v>0.241882324218749</v>
@@ -7386,7 +7007,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B66" s="8">
         <v>0.24219258626302001</v>
@@ -7409,7 +7030,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B67" s="8">
         <v>0.242462158203125</v>
@@ -7432,7 +7053,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B68" s="8">
         <v>0.24272664388020801</v>
@@ -7455,7 +7076,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B69" s="8">
         <v>0.24297078450520801</v>
@@ -7478,7 +7099,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B70" s="8">
         <v>0.25834147135416602</v>
@@ -7501,7 +7122,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B71" s="8">
         <v>0.27634684244791602</v>
@@ -7524,7 +7145,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B72" s="8">
         <v>0.29420979817708298</v>
@@ -7547,7 +7168,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B73" s="8">
         <v>0.311920166015625</v>
@@ -7570,7 +7191,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B74" s="8">
         <v>0.3294677734375</v>
@@ -7593,7 +7214,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B75" s="8">
         <v>0.3468017578125</v>
@@ -7616,7 +7237,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B76" s="8">
         <v>0.36388142903645798</v>
@@ -7639,7 +7260,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B77" s="8">
         <v>0.380752563476562</v>
@@ -7662,7 +7283,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B78" s="8">
         <v>0.39739481608072902</v>
@@ -7685,7 +7306,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B79" s="8">
         <v>0.41375223795572902</v>
@@ -7708,7 +7329,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B80" s="8">
         <v>0.42987060546875</v>
@@ -7731,7 +7352,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B81" s="8">
         <v>0.44578043619791602</v>
@@ -7754,7 +7375,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B82" s="8">
         <v>0.46132405598958298</v>
@@ -7777,7 +7398,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B83" s="8">
         <v>0.47652180989583298</v>
@@ -7800,7 +7421,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B84" s="8">
         <v>0.49140421549479102</v>
@@ -7823,7 +7444,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B85" s="8">
         <v>0.50583902994791596</v>
@@ -7846,7 +7467,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B86" s="8">
         <v>0.51984659830729096</v>
@@ -7869,7 +7490,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B87" s="8">
         <v>0.53346761067708304</v>
@@ -7892,7 +7513,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B88" s="8">
         <v>0.54660542805989498</v>
@@ -7915,7 +7536,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B89" s="8">
         <v>0.55940755208333304</v>
@@ -7938,7 +7559,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B90" s="8">
         <v>0.57175191243489498</v>
@@ -7961,7 +7582,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B91" s="8">
         <v>0.58357747395833304</v>
@@ -7984,7 +7605,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B92" s="8">
         <v>0.59494527180989498</v>
@@ -8007,7 +7628,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B93" s="8">
         <v>0.60578409830729096</v>
@@ -8030,7 +7651,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B94" s="8">
         <v>0.61615498860676998</v>
@@ -8053,7 +7674,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B95" s="8">
         <v>0.62605794270833304</v>
@@ -8076,7 +7697,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B96" s="8">
         <v>0.63542175292968694</v>
@@ -8099,7 +7720,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B97" s="8">
         <v>0.64417012532551998</v>
@@ -8122,7 +7743,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B98" s="8">
         <v>0.65254211425781194</v>
@@ -8145,7 +7766,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B99" s="8">
         <v>0.66028849283854096</v>
@@ -8168,7 +7789,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B100" s="8">
         <v>0.66762797037760402</v>
@@ -8191,7 +7812,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B101" s="8">
         <v>0.67443339029947902</v>
@@ -8214,7 +7835,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B102" s="8">
         <v>0.68081156412760402</v>
@@ -8237,7 +7858,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B103" s="8">
         <v>0.68663533528645804</v>
@@ -8260,7 +7881,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B104" s="8">
         <v>0.69193522135416596</v>
@@ -8283,7 +7904,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B105" s="8">
         <v>0.69670104980468694</v>
@@ -8306,7 +7927,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B106" s="8">
         <v>0.70102437337239498</v>
@@ -8329,7 +7950,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B107" s="8">
         <v>0.704864501953125</v>
@@ -8352,7 +7973,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B108" s="8">
         <v>0.708251953125</v>
@@ -8375,7 +7996,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B109" s="8">
         <v>0.71123758951822902</v>
@@ -8398,7 +8019,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B110" s="8">
         <v>0.713775634765625</v>
@@ -8421,7 +8042,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B111" s="8">
         <v>0.71602884928385402</v>
@@ -8444,7 +8065,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B112" s="8">
         <v>0.71789042154947902</v>
@@ -8467,7 +8088,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B113" s="8">
         <v>0.71936543782551998</v>
@@ -8490,7 +8111,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B114" s="8">
         <v>0.72064717610676998</v>
@@ -8513,7 +8134,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B115" s="8">
         <v>0.72159830729166596</v>
@@ -8536,7 +8157,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B116" s="8">
         <v>0.72222900390625</v>
@@ -8559,7 +8180,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B117" s="8">
         <v>0.72263081868489498</v>
@@ -8582,7 +8203,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B118" s="8">
         <v>0.74753316243489498</v>
@@ -8605,7 +8226,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B119" s="8">
         <v>0.77240498860677098</v>
@@ -8628,7 +8249,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B120" s="8">
         <v>0.79719543457031194</v>
@@ -8651,7 +8272,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B121" s="8">
         <v>0.82194010416666596</v>
@@ -8674,7 +8295,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B122" s="8">
         <v>0.84660339355468694</v>
@@ -8697,7 +8318,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B123" s="8">
         <v>0.87120564778645804</v>
@@ -8720,7 +8341,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B124" s="8">
         <v>0.89574178059895804</v>
@@ -8743,7 +8364,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B125" s="8">
         <v>0.92016092936197902</v>
@@ -8766,7 +8387,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B126" s="8">
         <v>0.94450378417968694</v>
@@ -8789,7 +8410,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B127" s="8">
         <v>0.968749999999999</v>
@@ -8812,7 +8433,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B128" s="8">
         <v>0.99284362792968694</v>
@@ -8835,7 +8456,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B129" s="8">
         <v>1.0167643229166601</v>
@@ -8858,7 +8479,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B130" s="8">
         <v>1.0404612223307199</v>
@@ -8881,7 +8502,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B131" s="8">
         <v>1.06391398111979</v>
@@ -8904,7 +8525,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B132" s="8">
         <v>1.08707173665364</v>
@@ -8927,7 +8548,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B133" s="8">
         <v>1.10983784993489</v>
@@ -8950,7 +8571,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B134" s="8">
         <v>1.13221232096354</v>
@@ -8973,7 +8594,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B135" s="8">
         <v>1.1541798909505201</v>
@@ -8996,7 +8617,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B136" s="8">
         <v>1.1756134033203101</v>
@@ -9019,7 +8640,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B137" s="8">
         <v>1.19633483886718</v>
@@ -9042,7 +8663,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B138" s="8">
         <v>1.2165476481119699</v>
@@ -9065,7 +8686,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B139" s="8">
         <v>1.23604838053385</v>
@@ -9088,7 +8709,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B140" s="8">
         <v>1.2549133300781199</v>
@@ -9111,7 +8732,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B141" s="8">
         <v>1.2731018066406199</v>
@@ -9134,7 +8755,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B142" s="8">
         <v>1.2906443277994699</v>
@@ -9157,7 +8778,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B143" s="8">
         <v>1.30756632486979</v>
@@ -9180,7 +8801,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B144" s="8">
         <v>1.3239034016927</v>
@@ -9203,7 +8824,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B145" s="8">
         <v>1.3395436604817701</v>
@@ -9226,7 +8847,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B146" s="8">
         <v>1.3544718424479101</v>
@@ -9249,7 +8870,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B147" s="8">
         <v>1.3687082926432199</v>
@@ -9272,7 +8893,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B148" s="8">
         <v>1.38217671712239</v>
@@ -9295,7 +8916,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B149" s="8">
         <v>1.3947296142578101</v>
@@ -9318,7 +8939,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B150" s="8">
         <v>1.4063313802083299</v>
@@ -9341,7 +8962,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B151" s="8">
         <v>1.4170481363932199</v>
@@ -9364,7 +8985,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B152" s="8">
         <v>1.42696634928385</v>
@@ -9387,7 +9008,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B153" s="8">
         <v>1.43600972493489</v>
@@ -9410,7 +9031,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B154" s="8">
         <v>1.4442443847656199</v>
@@ -9433,7 +9054,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B155" s="8">
         <v>1.45166015625</v>
@@ -9456,7 +9077,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B156" s="8">
         <v>1.45835876464843</v>
@@ -9479,7 +9100,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B157" s="8">
         <v>1.4642384847005201</v>
@@ -9502,7 +9123,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B158" s="8">
         <v>1.4694519042968699</v>
@@ -9525,7 +9146,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B159" s="8">
         <v>1.4738972981770799</v>
@@ -9548,7 +9169,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B160" s="8">
         <v>1.47779337565104</v>
@@ -9571,7 +9192,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B161" s="8">
         <v>1.4810587565104101</v>
@@ -9594,7 +9215,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B162" s="8">
         <v>1.48338317871093</v>
@@ -9617,7 +9238,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B163" s="8">
         <v>1.48455810546875</v>
@@ -9640,7 +9261,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B164" s="8">
         <v>1.4848836263020799</v>
@@ -9663,7 +9284,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B165" s="8">
         <v>1.4851481119791601</v>
@@ -9691,7 +9312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB8A61D-3EA8-4BBB-9246-E018E6EA153F}">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -10024,4 +9645,237 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59202079-AD42-4F5C-8E99-21070582FC6A}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA51" sqref="AA51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1.8E-3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.1415733333333333</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.37627519542972249</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.23470186209638921</v>
+      </c>
+      <c r="E2" s="2">
+        <v>29.014907360076901</v>
+      </c>
+      <c r="F2" s="2">
+        <v>29.01263125737508</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.2761027018241009E-3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.93290496369202935</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.93289164702097571</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.331667105364254E-5</v>
+      </c>
+      <c r="K2" s="6">
+        <v>112.79812878575019</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.28842345873514807</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.36777948091427493</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.218496</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.45518568033973378</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.23668968033973381</v>
+      </c>
+      <c r="E3" s="2">
+        <v>30.542146682739261</v>
+      </c>
+      <c r="F3" s="2">
+        <v>30.538185516993209</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.9611657460518757E-3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.95307789742946625</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.95306503772735596</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.2859702110290531E-5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>81.505320350226839</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.22515885035196939</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.31315292914708448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.32326933333333341</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.55609557777643204</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.23282624444309871</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32.069103717803962</v>
+      </c>
+      <c r="F4" s="2">
+        <v>32.06329027811686</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5.8134396870954666E-3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.96799124032258987</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.96797890961170197</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.2330710887908941E-5</v>
+      </c>
+      <c r="K4" s="6">
+        <v>53.088313848355369</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.16271258393923441</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.25484423339366907</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.69234133333333314</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.90979902197917306</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.21745768864583989</v>
+      </c>
+      <c r="E5" s="2">
+        <v>35.652261098225907</v>
+      </c>
+      <c r="F5" s="2">
+        <v>35.640590826670334</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.1670271555587419E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.98580639561017358</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.98580269267161691</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3.702938556671143E-6</v>
+      </c>
+      <c r="K5" s="6">
+        <v>21.816504512335481</v>
+      </c>
+      <c r="L5" s="6">
+        <v>8.5436006387074784E-2</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.154677485426267</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a New Model
</commit_message>
<xml_diff>
--- a/Evaluation Result/xlsx/Evaluation.xlsx
+++ b/Evaluation Result/xlsx/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\Learned-Image-Compression\Evaluation Result\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B10CE03-F240-40C9-807A-0B51F4B0C427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72AE41F-717D-465C-B1CA-49D334C1F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="868" activeTab="6" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
+    <workbookView xWindow="-15098" yWindow="-4358" windowWidth="15196" windowHeight="23476" tabRatio="868" firstSheet="12" activeTab="17" xr2:uid="{B8EB7B44-9B16-4AE5-9F61-DEDF5636CF32}"/>
   </bookViews>
   <sheets>
     <sheet name="Factorized" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="CCA2024" sheetId="33" r:id="rId15"/>
     <sheet name="WeConvene2024" sheetId="39" r:id="rId16"/>
     <sheet name="FTIC2024" sheetId="35" r:id="rId17"/>
+    <sheet name="STanH" sheetId="42" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="185">
   <si>
     <t>Δms-ssim</t>
   </si>
@@ -606,6 +607,13 @@
   </si>
   <si>
     <t>bpp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Derivation</t>
+  </si>
+  <si>
+    <t>Anchor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3843,6 +3851,383 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3463CEDE-AE96-4DDB-B2B9-3D178A001B96}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.125" style="4" customWidth="1"/>
+    <col min="2" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.75" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.260041666666666</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.26220833333333299</v>
+      </c>
+      <c r="D2" s="3">
+        <f>ABS(B2-C2)</f>
+        <v>2.1666666666669832E-3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>30.481266666666599</v>
+      </c>
+      <c r="F2" s="2">
+        <v>30.4813875</v>
+      </c>
+      <c r="G2" s="3">
+        <f>ABS(E2-F2)</f>
+        <v>1.2083333340129343E-4</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.95783188703324751</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.95783868318231002</v>
+      </c>
+      <c r="J2" s="3">
+        <f>ABS(H2-I2)</f>
+        <v>6.7961490625156884E-6</v>
+      </c>
+      <c r="K2" s="6">
+        <v>56.4115757037601</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.12569092710812799</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.29268127679824801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.31512499999999999</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.31479166666666603</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D8" si="0">ABS(B3-C3)</f>
+        <v>3.3333333333396276E-4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>31.695645833333302</v>
+      </c>
+      <c r="F3" s="2">
+        <v>31.695591666666601</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G8" si="1">ABS(E3-F3)</f>
+        <v>5.4166666700439237E-5</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.96800254649539308</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.96800355953617379</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J8" si="2">ABS(H3-I3)</f>
+        <v>1.013040780706298E-6</v>
+      </c>
+      <c r="K3" s="6">
+        <v>48.491065844448002</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.10248064994812001</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.25651100029548002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.36033333333333301</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.35845833333333299</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8750000000000155E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>32.419795833333303</v>
+      </c>
+      <c r="F4" s="2">
+        <v>32.419787499999899</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3333334046642449E-6</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.97280397594317813</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.97280183630272876</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="2"/>
+        <v>2.1396404493723153E-6</v>
+      </c>
+      <c r="K4" s="6">
+        <v>43.170418048674598</v>
+      </c>
+      <c r="L4" s="6">
+        <v>9.0161482493082604E-2</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0.235784205297629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.43566666666666598</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.43179166666666602</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>3.8749999999999618E-3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>33.344595833333301</v>
+      </c>
+      <c r="F5" s="2">
+        <v>33.344929166666603</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3333333330176629E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.97796238542019631</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.97796957290792075</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="2"/>
+        <v>7.1874877244360036E-6</v>
+      </c>
+      <c r="K5" s="6">
+        <v>36.819434291220396</v>
+      </c>
+      <c r="L5" s="6">
+        <v>7.5220733880996704E-2</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0.21415686359008099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.51170833333333299</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.50679166666666597</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>4.9166666666670134E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>33.996720833333299</v>
+      </c>
+      <c r="F6" s="2">
+        <v>33.996600000000001</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2083333329826473E-4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.9810897944309005</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.98108836110731679</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4333235837105107E-6</v>
+      </c>
+      <c r="K6" s="6">
+        <v>32.731103179490503</v>
+      </c>
+      <c r="L6" s="6">
+        <v>6.6387926538785294E-2</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0.20101573814948401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.646708333333333</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.63949999999999996</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>7.2083333333330391E-3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>34.664429166666601</v>
+      </c>
+      <c r="F7" s="2">
+        <v>34.664066666666599</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
+        <v>3.6250000000137561E-4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.98374610312450339</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.98374541696704199</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="2"/>
+        <v>6.861574614047683E-7</v>
+      </c>
+      <c r="K7" s="6">
+        <v>31.0610796468515</v>
+      </c>
+      <c r="L7" s="6">
+        <v>6.0380990306536299E-2</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0.19403065492709401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.71475</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.706666666666666</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>8.0833333333339974E-3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>34.841862499999998</v>
+      </c>
+      <c r="F8" s="2">
+        <v>34.841491666666599</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7083333339893443E-4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.98440402608997746</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.98440200596219818</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="2"/>
+        <v>2.0201277792786243E-6</v>
+      </c>
+      <c r="K8" s="6">
+        <v>30.2891943100195</v>
+      </c>
+      <c r="L8" s="6">
+        <v>5.8884814381599399E-2</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0.19218107809623</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF463B40-663A-4815-B646-230C55393493}">
   <dimension ref="A1:N9"/>
@@ -5735,7 +6120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78BAAE4-DD50-43F7-995D-5556F000B121}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8:J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>